<commit_message>
Update CSSECDV - Case Study 1 Project Documentation.xlsx
</commit_message>
<xml_diff>
--- a/CSSECDV - Case Study 1 Project Documentation.xlsx
+++ b/CSSECDV - Case Study 1 Project Documentation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\school\AY 2022-2023\term 3\cssecdv\case study\cs1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aurelio Garcia\Documents\IntelliJPrograms\cssecdv-cs1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26D9D9F-B2EF-4BB4-ADF9-947B95BCB741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B00FC47-83E2-4E77-BB24-C748C780F49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{E5B6E951-E296-6A45-B171-4DEF88B6BA8E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E5B6E951-E296-6A45-B171-4DEF88B6BA8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Security Issue</t>
   </si>
@@ -125,6 +125,18 @@
   </si>
   <si>
     <t>Created a method that flashes a statement that either the username or password is incorrect ("Username or password is incorrect"), which was called in the loginAction method in Frame.java</t>
+  </si>
+  <si>
+    <t>Updating passwords</t>
+  </si>
+  <si>
+    <t>Login.java, Frame.java, ResetRequest.java, ResetPassword.java</t>
+  </si>
+  <si>
+    <t>No chance to reset password. If resetting password is allowed and no controls, attackers could reset password whenever wanted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When a password reset is requested, the user must input their email. A reset code (dummy) is sent to their email (dummy). They must then input that reset code, their new password, and their confirmed new password to change their password. </t>
   </si>
 </sst>
 </file>
@@ -665,23 +677,23 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="40.875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="20.875" style="13" customWidth="1"/>
-    <col min="4" max="4" width="40.875" style="13" customWidth="1"/>
-    <col min="5" max="5" width="60.875" style="13" customWidth="1"/>
+    <col min="1" max="1" width="7.59765625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="40.8984375" style="13" customWidth="1"/>
+    <col min="3" max="3" width="20.8984375" style="13" customWidth="1"/>
+    <col min="4" max="4" width="40.8984375" style="13" customWidth="1"/>
+    <col min="5" max="5" width="60.8984375" style="13" customWidth="1"/>
     <col min="6" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
@@ -698,7 +710,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="78" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -715,7 +727,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -732,7 +744,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -749,7 +761,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -766,7 +778,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -783,16 +795,24 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -801,7 +821,7 @@
       <c r="D8" s="6"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -810,7 +830,7 @@
       <c r="D9" s="6"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -819,7 +839,7 @@
       <c r="D10" s="6"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -828,7 +848,7 @@
       <c r="D11" s="6"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -837,7 +857,7 @@
       <c r="D12" s="6"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -846,7 +866,7 @@
       <c r="D13" s="6"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -855,7 +875,7 @@
       <c r="D14" s="6"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -864,7 +884,7 @@
       <c r="D15" s="6"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -873,7 +893,7 @@
       <c r="D16" s="6"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>15</v>
       </c>
@@ -882,7 +902,7 @@
       <c r="D17" s="6"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -891,7 +911,7 @@
       <c r="D18" s="6"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>17</v>
       </c>
@@ -900,7 +920,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -909,7 +929,7 @@
       <c r="D20" s="6"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>19</v>
       </c>
@@ -918,7 +938,7 @@
       <c r="D21" s="6"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Documentation: added lockout, unauthorized access, weak passwords, and unhashed passwords
</commit_message>
<xml_diff>
--- a/CSSECDV - Case Study 1 Project Documentation.xlsx
+++ b/CSSECDV - Case Study 1 Project Documentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aurelio Garcia\Documents\IntelliJPrograms\cssecdv-cs1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\cssecdv-cs1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B00FC47-83E2-4E77-BB24-C748C780F49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838E407C-D814-414D-8A06-4401D59F814D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E5B6E951-E296-6A45-B171-4DEF88B6BA8E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11040" xr2:uid="{E5B6E951-E296-6A45-B171-4DEF88B6BA8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>Security Issue</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>Register.java, Frame.java</t>
-  </si>
-  <si>
-    <t>A user mistyping theit password may unintentionally create an account with a different password, which can lead to confusion or potential security breaches.</t>
   </si>
   <si>
     <t>Created a method that flashes a statement that the passwords are mismatched. Which was called in the registerAction method in Frame.java if the password and confpass are not equal.
@@ -137,6 +134,51 @@
   </si>
   <si>
     <t xml:space="preserve">When a password reset is requested, the user must input their email. A reset code (dummy) is sent to their email (dummy). They must then input that reset code, their new password, and their confirmed new password to change their password. </t>
+  </si>
+  <si>
+    <t>No account lockout policy</t>
+  </si>
+  <si>
+    <t>Having no lockout policy for multiple attempts at logging into an account leads to the possibility of unauthorized user access through brute force methods.</t>
+  </si>
+  <si>
+    <t>Lock the account after a specified number of unsuccessful login attempts. Each unsuccessful attempt is logged in the Logs Arraylist and after five failed attempts, the locked status of the account is set to '1'. An error message is displayed notifying the user that the account they are trying to access is locked.</t>
+  </si>
+  <si>
+    <t>Unauthorized access to information and actions</t>
+  </si>
+  <si>
+    <t>Frame.java</t>
+  </si>
+  <si>
+    <t>Unauthorized users can manipulate information and perform actions that they originally do not have the privilege to.</t>
+  </si>
+  <si>
+    <t>Make use of the Role Codes and use it to designate the proper management page that they have access to. A user with a role code of '2' should only be able to access the client page, while an admin whose role code is '5' should be able access the admin page.</t>
+  </si>
+  <si>
+    <t>Weak Passwords</t>
+  </si>
+  <si>
+    <t>Weak passwords, typically short or simple ones, are more susceptible to brute force attacks. In a brute force attack, an attacker systematically tries all possible combinations of passwords until the correct one is found.</t>
+  </si>
+  <si>
+    <t>Enforce a strict password requirement that would decrease the odds of having attackers brute force their way into figuring out the combination. Such practices would involve including a minimum character limit, requirement of uppercase and lowercase letters, numerical digits, and sepcial characters.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frame.java, Register.java, Login.java, ResetPassword.java </t>
+  </si>
+  <si>
+    <t>Improperly hashed passwords that are stored in the database allows attackers to easily input a user's password without having to decrypt them if they somehow gained access to the database.</t>
+  </si>
+  <si>
+    <t>Implement a hashing algorithm for passwords when stored in the database. This also keeps the passwords of the users confidential and protects them from being easily accessed.</t>
+  </si>
+  <si>
+    <t>A user mistyping their password may unintentionally create an account with a different password, which can lead to confusion or potential security breaches.</t>
+  </si>
+  <si>
+    <t>Unhashed Passwords</t>
   </si>
 </sst>
 </file>
@@ -677,23 +719,23 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.59765625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="40.8984375" style="13" customWidth="1"/>
-    <col min="3" max="3" width="20.8984375" style="13" customWidth="1"/>
-    <col min="4" max="4" width="40.8984375" style="13" customWidth="1"/>
-    <col min="5" max="5" width="60.8984375" style="13" customWidth="1"/>
+    <col min="1" max="1" width="7.625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="40.875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="20.875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="40.875" style="13" customWidth="1"/>
+    <col min="5" max="5" width="60.875" style="13" customWidth="1"/>
     <col min="6" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
@@ -710,7 +752,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="78" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -727,7 +769,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -744,7 +786,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -755,100 +797,132 @@
         <v>15</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:5" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>9</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -857,7 +931,7 @@
       <c r="D12" s="6"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -866,7 +940,7 @@
       <c r="D13" s="6"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -875,7 +949,7 @@
       <c r="D14" s="6"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -884,7 +958,7 @@
       <c r="D15" s="6"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -893,7 +967,7 @@
       <c r="D16" s="6"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>15</v>
       </c>
@@ -902,7 +976,7 @@
       <c r="D17" s="6"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -911,7 +985,7 @@
       <c r="D18" s="6"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>17</v>
       </c>
@@ -920,7 +994,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -929,7 +1003,7 @@
       <c r="D20" s="6"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>19</v>
       </c>
@@ -938,7 +1012,7 @@
       <c r="D21" s="6"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>20</v>
       </c>

</xml_diff>